<commit_message>
Add instructions worksheet to xlsx file. So far empty.
</commit_message>
<xml_diff>
--- a/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
+++ b/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
@@ -7,10 +7,11 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="experiment" sheetId="1" r:id="rId1"/>
-    <sheet name="cv_experiment" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="run" sheetId="3" r:id="rId3"/>
-    <sheet name="cv_run" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="experiment" sheetId="2" r:id="rId2"/>
+    <sheet name="cv_experiment" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="run" sheetId="4" r:id="rId4"/>
+    <sheet name="cv_run" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="filetype">'cv_run'!$C$1:$C$24</definedName>
@@ -25,7 +26,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="246">
+  <si>
+    <t>Instructions how to fill the metadata template</t>
+  </si>
   <si>
     <t>alias</t>
   </si>
@@ -1105,7 +1109,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1114,92 +1118,113 @@
     <col min="1" max="301" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="301" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="150" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="G1:N83"/>
   <sheetViews>
@@ -1234,711 +1259,711 @@
   <sheetData>
     <row r="1" spans="7:14">
       <c r="G1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="7:14">
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="7:14">
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="7:14">
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="7:14">
       <c r="G5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="7:14">
       <c r="G6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="7:14">
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="7:14">
       <c r="G8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="7:14">
       <c r="G9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="7:14">
       <c r="G10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="7:14">
       <c r="G11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="7:14">
       <c r="G12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="7:14">
       <c r="G13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="7:14">
       <c r="G14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="7:14">
       <c r="G15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="7:14">
       <c r="G16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="7:14">
       <c r="G17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="7:14">
       <c r="G18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="7:14">
       <c r="G19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="7:14">
       <c r="G20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="7:14">
       <c r="G21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="7:14">
       <c r="G22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="7:14">
       <c r="G23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="7:14">
       <c r="G24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="7:14">
       <c r="G25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="7:14">
       <c r="G26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="7:14">
       <c r="G27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="7:14">
       <c r="G28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="7:14">
       <c r="G29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="7:14">
       <c r="G30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="7:14">
       <c r="G31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="7:14">
       <c r="G32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="7:14">
       <c r="G33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="7:14">
       <c r="G34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="7:14">
       <c r="G35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="7:14">
       <c r="G36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="7:14">
       <c r="G37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="7:14">
       <c r="G38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="7:14">
       <c r="G39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="7:14">
       <c r="G40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="7:14">
       <c r="G41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="7:14">
       <c r="N42" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="7:14">
       <c r="N43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="7:14">
       <c r="N44" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="7:14">
       <c r="N45" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="7:14">
       <c r="N46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="7:14">
       <c r="N47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="7:14">
       <c r="N48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="14:14">
       <c r="N49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="14:14">
       <c r="N50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="14:14">
       <c r="N51" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="14:14">
       <c r="N52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="14:14">
       <c r="N53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="14:14">
       <c r="N54" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="14:14">
       <c r="N55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="14:14">
       <c r="N56" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="14:14">
       <c r="N57" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="14:14">
       <c r="N58" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="14:14">
       <c r="N59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="14:14">
       <c r="N60" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="14:14">
       <c r="N61" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="14:14">
       <c r="N62" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="14:14">
       <c r="N63" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="14:14">
       <c r="N64" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="14:14">
       <c r="N65" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="14:14">
       <c r="N66" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="14:14">
       <c r="N67" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="14:14">
       <c r="N68" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="14:14">
       <c r="N69" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="14:14">
       <c r="N70" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="14:14">
       <c r="N71" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="14:14">
       <c r="N72" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="14:14">
       <c r="N73" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="14:14">
       <c r="N74" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="14:14">
       <c r="N75" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="14:14">
       <c r="N76" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="14:14">
       <c r="N77" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="14:14">
       <c r="N78" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="14:14">
       <c r="N79" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="14:14">
       <c r="N80" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="14:14">
       <c r="N81" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" spans="14:14">
       <c r="N82" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="14:14">
       <c r="N83" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1946,7 +1971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1959,60 +1984,60 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="150" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2025,7 +2050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:C24"/>
   <sheetViews>
@@ -2035,122 +2060,122 @@
   <sheetData>
     <row r="1" spans="3:3">
       <c r="C1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove platform field from ENA, since it is non-mandatory when specifying instrument_model
</commit_message>
<xml_diff>
--- a/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
+++ b/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
@@ -15,18 +15,17 @@
   </sheets>
   <definedNames>
     <definedName name="filetype">'cv_run'!$C$1:$C$24</definedName>
-    <definedName name="instrumentmodel">'cv_experiment'!$N$1:$N$83</definedName>
+    <definedName name="instrumentmodel">'cv_experiment'!$M$1:$M$83</definedName>
     <definedName name="libraryselection">'cv_experiment'!$I$1:$I$31</definedName>
     <definedName name="librarysource">'cv_experiment'!$H$1:$H$9</definedName>
     <definedName name="librarystrategy">'cv_experiment'!$G$1:$G$41</definedName>
-    <definedName name="platform">'cv_experiment'!$M$1:$M$17</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="227">
   <si>
     <t>Instructions how to fill the metadata template</t>
   </si>
@@ -338,63 +337,6 @@
   </si>
   <si>
     <t>(Optional) Free form text describing the protocol by which the sequencing library was constructed.</t>
-  </si>
-  <si>
-    <t>LS454</t>
-  </si>
-  <si>
-    <t>ILLUMINA</t>
-  </si>
-  <si>
-    <t>HELICOS</t>
-  </si>
-  <si>
-    <t>ABI_SOLID</t>
-  </si>
-  <si>
-    <t>COMPLETE_GENOMICS</t>
-  </si>
-  <si>
-    <t>BGISEQ</t>
-  </si>
-  <si>
-    <t>OXFORD_NANOPORE</t>
-  </si>
-  <si>
-    <t>PACBIO_SMRT</t>
-  </si>
-  <si>
-    <t>ION_TORRENT</t>
-  </si>
-  <si>
-    <t>CAPILLARY</t>
-  </si>
-  <si>
-    <t>DNBSEQ</t>
-  </si>
-  <si>
-    <t>ELEMENT</t>
-  </si>
-  <si>
-    <t>ULTIMA</t>
-  </si>
-  <si>
-    <t>VELA_DIAGNOSTICS</t>
-  </si>
-  <si>
-    <t>GENAPSYS</t>
-  </si>
-  <si>
-    <t>GENEMIND</t>
-  </si>
-  <si>
-    <t>TAPESTRI</t>
-  </si>
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>(Mandatory) The platform record selects which sequencing platform and platform-specific runtime parameters. this will be determined by the center. optional if 'instrument_model' is provided.</t>
   </si>
   <si>
     <t>454 GS</t>
@@ -1130,7 +1072,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1139,7 +1081,7 @@
     <col min="1" max="301" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1177,13 +1119,10 @@
         <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="150" customHeight="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="150" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1221,14 +1160,11 @@
         <v>103</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G101">
       <formula1>librarystrategy</formula1>
     </dataValidation>
@@ -1239,9 +1175,6 @@
       <formula1>libraryselection</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M101">
-      <formula1>platform</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N101">
       <formula1>instrumentmodel</formula1>
     </dataValidation>
   </dataValidations>
@@ -1251,13 +1184,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="G1:N83"/>
+  <dimension ref="G1:M83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="7:14">
+    <row r="1" spans="7:13">
       <c r="G1" t="s">
         <v>13</v>
       </c>
@@ -1270,11 +1203,8 @@
       <c r="M1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="7:14">
+    </row>
+    <row r="2" spans="7:13">
       <c r="G2" t="s">
         <v>14</v>
       </c>
@@ -1287,11 +1217,8 @@
       <c r="M2" t="s">
         <v>105</v>
       </c>
-      <c r="N2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="7:14">
+    </row>
+    <row r="3" spans="7:13">
       <c r="G3" t="s">
         <v>15</v>
       </c>
@@ -1304,11 +1231,8 @@
       <c r="M3" t="s">
         <v>106</v>
       </c>
-      <c r="N3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="7:14">
+    </row>
+    <row r="4" spans="7:13">
       <c r="G4" t="s">
         <v>16</v>
       </c>
@@ -1321,11 +1245,8 @@
       <c r="M4" t="s">
         <v>107</v>
       </c>
-      <c r="N4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="7:14">
+    </row>
+    <row r="5" spans="7:13">
       <c r="G5" t="s">
         <v>17</v>
       </c>
@@ -1338,11 +1259,8 @@
       <c r="M5" t="s">
         <v>108</v>
       </c>
-      <c r="N5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="7:14">
+    </row>
+    <row r="6" spans="7:13">
       <c r="G6" t="s">
         <v>18</v>
       </c>
@@ -1355,11 +1273,8 @@
       <c r="M6" t="s">
         <v>109</v>
       </c>
-      <c r="N6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="7:14">
+    </row>
+    <row r="7" spans="7:13">
       <c r="G7" t="s">
         <v>19</v>
       </c>
@@ -1372,11 +1287,8 @@
       <c r="M7" t="s">
         <v>110</v>
       </c>
-      <c r="N7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="7:14">
+    </row>
+    <row r="8" spans="7:13">
       <c r="G8" t="s">
         <v>20</v>
       </c>
@@ -1389,11 +1301,8 @@
       <c r="M8" t="s">
         <v>111</v>
       </c>
-      <c r="N8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="7:14">
+    </row>
+    <row r="9" spans="7:13">
       <c r="G9" t="s">
         <v>21</v>
       </c>
@@ -1406,11 +1315,8 @@
       <c r="M9" t="s">
         <v>112</v>
       </c>
-      <c r="N9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="7:14">
+    </row>
+    <row r="10" spans="7:13">
       <c r="G10" t="s">
         <v>22</v>
       </c>
@@ -1420,11 +1326,8 @@
       <c r="M10" t="s">
         <v>113</v>
       </c>
-      <c r="N10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="7:14">
+    </row>
+    <row r="11" spans="7:13">
       <c r="G11" t="s">
         <v>23</v>
       </c>
@@ -1434,11 +1337,8 @@
       <c r="M11" t="s">
         <v>114</v>
       </c>
-      <c r="N11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="7:14">
+    </row>
+    <row r="12" spans="7:13">
       <c r="G12" t="s">
         <v>24</v>
       </c>
@@ -1448,11 +1348,8 @@
       <c r="M12" t="s">
         <v>115</v>
       </c>
-      <c r="N12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="7:14">
+    </row>
+    <row r="13" spans="7:13">
       <c r="G13" t="s">
         <v>25</v>
       </c>
@@ -1462,11 +1359,8 @@
       <c r="M13" t="s">
         <v>116</v>
       </c>
-      <c r="N13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="7:14">
+    </row>
+    <row r="14" spans="7:13">
       <c r="G14" t="s">
         <v>26</v>
       </c>
@@ -1476,11 +1370,8 @@
       <c r="M14" t="s">
         <v>117</v>
       </c>
-      <c r="N14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="7:14">
+    </row>
+    <row r="15" spans="7:13">
       <c r="G15" t="s">
         <v>27</v>
       </c>
@@ -1490,11 +1381,8 @@
       <c r="M15" t="s">
         <v>118</v>
       </c>
-      <c r="N15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="7:14">
+    </row>
+    <row r="16" spans="7:13">
       <c r="G16" t="s">
         <v>28</v>
       </c>
@@ -1504,11 +1392,8 @@
       <c r="M16" t="s">
         <v>119</v>
       </c>
-      <c r="N16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="7:14">
+    </row>
+    <row r="17" spans="7:13">
       <c r="G17" t="s">
         <v>29</v>
       </c>
@@ -1518,451 +1403,448 @@
       <c r="M17" t="s">
         <v>120</v>
       </c>
-      <c r="N17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="7:14">
+    </row>
+    <row r="18" spans="7:13">
       <c r="G18" t="s">
         <v>30</v>
       </c>
       <c r="I18" t="s">
         <v>32</v>
       </c>
-      <c r="N18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="7:14">
+      <c r="M18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="7:13">
       <c r="G19" t="s">
         <v>31</v>
       </c>
       <c r="I19" t="s">
         <v>83</v>
       </c>
-      <c r="N19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="7:14">
+      <c r="M19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="7:13">
       <c r="G20" t="s">
         <v>32</v>
       </c>
       <c r="I20" t="s">
         <v>84</v>
       </c>
-      <c r="N20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="7:14">
+      <c r="M20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="7:13">
       <c r="G21" t="s">
         <v>33</v>
       </c>
       <c r="I21" t="s">
         <v>85</v>
       </c>
-      <c r="N21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="7:14">
+      <c r="M21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="7:13">
       <c r="G22" t="s">
         <v>34</v>
       </c>
       <c r="I22" t="s">
         <v>86</v>
       </c>
-      <c r="N22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="7:14">
+      <c r="M22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="7:13">
       <c r="G23" t="s">
         <v>35</v>
       </c>
       <c r="I23" t="s">
         <v>87</v>
       </c>
-      <c r="N23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="7:14">
+      <c r="M23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="7:13">
       <c r="G24" t="s">
         <v>36</v>
       </c>
       <c r="I24" t="s">
         <v>88</v>
       </c>
-      <c r="N24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="7:14">
+      <c r="M24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="7:13">
       <c r="G25" t="s">
         <v>37</v>
       </c>
       <c r="I25" t="s">
         <v>89</v>
       </c>
-      <c r="N25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="7:14">
+      <c r="M25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="7:13">
       <c r="G26" t="s">
         <v>38</v>
       </c>
       <c r="I26" t="s">
         <v>90</v>
       </c>
-      <c r="N26" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="7:14">
+      <c r="M26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="7:13">
       <c r="G27" t="s">
         <v>39</v>
       </c>
       <c r="I27" t="s">
         <v>91</v>
       </c>
-      <c r="N27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="7:14">
+      <c r="M27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="7:13">
       <c r="G28" t="s">
         <v>40</v>
       </c>
       <c r="I28" t="s">
         <v>92</v>
       </c>
-      <c r="N28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="7:14">
+      <c r="M28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="7:13">
       <c r="G29" t="s">
         <v>41</v>
       </c>
       <c r="I29" t="s">
         <v>93</v>
       </c>
-      <c r="N29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="7:14">
+      <c r="M29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="7:13">
       <c r="G30" t="s">
         <v>42</v>
       </c>
       <c r="I30" t="s">
         <v>94</v>
       </c>
-      <c r="N30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="7:14">
+      <c r="M30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="7:13">
       <c r="G31" t="s">
         <v>43</v>
       </c>
       <c r="I31" t="s">
         <v>95</v>
       </c>
-      <c r="N31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="7:14">
+      <c r="M31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="7:13">
       <c r="G32" t="s">
         <v>44</v>
       </c>
-      <c r="N32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="7:14">
+      <c r="M32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="7:13">
       <c r="G33" t="s">
         <v>45</v>
       </c>
-      <c r="N33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="7:14">
+      <c r="M33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="7:13">
       <c r="G34" t="s">
         <v>46</v>
       </c>
-      <c r="N34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="7:14">
+      <c r="M34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="7:13">
       <c r="G35" t="s">
         <v>47</v>
       </c>
-      <c r="N35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="7:14">
+      <c r="M35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="7:13">
       <c r="G36" t="s">
         <v>48</v>
       </c>
-      <c r="N36" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="7:14">
+      <c r="M36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="7:13">
       <c r="G37" t="s">
         <v>49</v>
       </c>
-      <c r="N37" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="7:14">
+      <c r="M37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="7:13">
       <c r="G38" t="s">
         <v>50</v>
       </c>
-      <c r="N38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="7:14">
+      <c r="M38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="7:13">
       <c r="G39" t="s">
         <v>51</v>
       </c>
-      <c r="N39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="7:14">
+      <c r="M39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="7:13">
       <c r="G40" t="s">
         <v>52</v>
       </c>
-      <c r="N40" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="7:14">
+      <c r="M40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="7:13">
       <c r="G41" t="s">
         <v>53</v>
       </c>
-      <c r="N41" t="s">
+      <c r="M41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="7:13">
+      <c r="M42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="7:13">
+      <c r="M43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="7:13">
+      <c r="M44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="7:13">
+      <c r="M45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="7:13">
+      <c r="M46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="7:13">
+      <c r="M47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="7:13">
+      <c r="M48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="13:13">
+      <c r="M49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="13:13">
+      <c r="M50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="13:13">
+      <c r="M51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="13:13">
+      <c r="M52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="13:13">
+      <c r="M53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="13:13">
+      <c r="M54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="13:13">
+      <c r="M55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="13:13">
+      <c r="M56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="13:13">
+      <c r="M57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="13:13">
+      <c r="M58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="13:13">
+      <c r="M59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="13:13">
+      <c r="M60" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="7:14">
-      <c r="N42" t="s">
+    <row r="61" spans="13:13">
+      <c r="M61" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="7:14">
-      <c r="N43" t="s">
+    <row r="62" spans="13:13">
+      <c r="M62" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="7:14">
-      <c r="N44" t="s">
+    <row r="63" spans="13:13">
+      <c r="M63" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="7:14">
-      <c r="N45" t="s">
+    <row r="64" spans="13:13">
+      <c r="M64" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="7:14">
-      <c r="N46" t="s">
+    <row r="65" spans="13:13">
+      <c r="M65" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="7:14">
-      <c r="N47" t="s">
+    <row r="66" spans="13:13">
+      <c r="M66" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="7:14">
-      <c r="N48" t="s">
+    <row r="67" spans="13:13">
+      <c r="M67" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="14:14">
-      <c r="N49" t="s">
+    <row r="68" spans="13:13">
+      <c r="M68" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="14:14">
-      <c r="N50" t="s">
+    <row r="69" spans="13:13">
+      <c r="M69" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="14:14">
-      <c r="N51" t="s">
+    <row r="70" spans="13:13">
+      <c r="M70" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="14:14">
-      <c r="N52" t="s">
+    <row r="71" spans="13:13">
+      <c r="M71" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="14:14">
-      <c r="N53" t="s">
+    <row r="72" spans="13:13">
+      <c r="M72" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="14:14">
-      <c r="N54" t="s">
+    <row r="73" spans="13:13">
+      <c r="M73" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="14:14">
-      <c r="N55" t="s">
+    <row r="74" spans="13:13">
+      <c r="M74" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="56" spans="14:14">
-      <c r="N56" t="s">
+    <row r="75" spans="13:13">
+      <c r="M75" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="14:14">
-      <c r="N57" t="s">
+    <row r="76" spans="13:13">
+      <c r="M76" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="14:14">
-      <c r="N58" t="s">
+    <row r="77" spans="13:13">
+      <c r="M77" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="14:14">
-      <c r="N59" t="s">
+    <row r="78" spans="13:13">
+      <c r="M78" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
-      <c r="N60" t="s">
+    <row r="79" spans="13:13">
+      <c r="M79" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="14:14">
-      <c r="N61" t="s">
+    <row r="80" spans="13:13">
+      <c r="M80" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="14:14">
-      <c r="N62" t="s">
+    <row r="81" spans="13:13">
+      <c r="M81" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="14:14">
-      <c r="N63" t="s">
+    <row r="82" spans="13:13">
+      <c r="M82" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="14:14">
-      <c r="N64" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="65" spans="14:14">
-      <c r="N65" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="14:14">
-      <c r="N66" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="14:14">
-      <c r="N67" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="68" spans="14:14">
-      <c r="N68" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="69" spans="14:14">
-      <c r="N69" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="70" spans="14:14">
-      <c r="N70" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="71" spans="14:14">
-      <c r="N71" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="72" spans="14:14">
-      <c r="N72" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="73" spans="14:14">
-      <c r="N73" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="74" spans="14:14">
-      <c r="N74" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="75" spans="14:14">
-      <c r="N75" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="76" spans="14:14">
-      <c r="N76" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="77" spans="14:14">
-      <c r="N77" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="78" spans="14:14">
-      <c r="N78" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="79" spans="14:14">
-      <c r="N79" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="80" spans="14:14">
-      <c r="N80" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="81" spans="14:14">
-      <c r="N81" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="82" spans="14:14">
-      <c r="N82" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="83" spans="14:14">
-      <c r="N83" t="s">
+    <row r="83" spans="13:13">
+      <c r="M83" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1987,57 +1869,57 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="150" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2060,122 +1942,122 @@
   <sheetData>
     <row r="1" spans="3:3">
       <c r="C1" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spell out cv as controlled_vocabulary
</commit_message>
<xml_diff>
--- a/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
+++ b/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="filetype">'cv_run'!$C$1:$C$24</definedName>
-    <definedName name="instrumentmodel">'cv_experiment'!$M$1:$M$83</definedName>
+    <definedName name="instrumentmodel">'cv_experiment'!$M$1:$M$85</definedName>
     <definedName name="libraryselection">'cv_experiment'!$I$1:$I$31</definedName>
     <definedName name="librarysource">'cv_experiment'!$H$1:$H$9</definedName>
     <definedName name="librarystrategy">'cv_experiment'!$G$1:$G$41</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="229">
   <si>
     <t>Instructions how to fill the metadata template</t>
   </si>
@@ -426,6 +426,9 @@
     <t>DNBSEQ-G50</t>
   </si>
   <si>
+    <t>DNBSEQ-T10x4RS</t>
+  </si>
+  <si>
     <t>DNBSEQ-T7</t>
   </si>
   <si>
@@ -505,6 +508,9 @@
   </si>
   <si>
     <t>Illumina NovaSeq X</t>
+  </si>
+  <si>
+    <t>Illumina NovaSeq X Plus</t>
   </si>
   <si>
     <t>Illumina iSeq 100</t>
@@ -1119,7 +1125,7 @@
         <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="150" customHeight="1">
@@ -1160,7 +1166,7 @@
         <v>103</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="G1:M83"/>
+  <dimension ref="G1:M85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1845,6 +1851,16 @@
     </row>
     <row r="83" spans="13:13">
       <c r="M83" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="13:13">
+      <c r="M84" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="13:13">
+      <c r="M85" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1869,57 +1885,57 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="150" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1942,122 +1958,122 @@
   <sheetData>
     <row r="1" spans="3:3">
       <c r="C1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add json template files (#24)
* Reformat organisational metadata files to be consistent with ENA_target_metadata_fields.yml

* Output genomics template as json

* first suggestion for a yaml file with internal info like version

* Refactor I/O code

* Base json template file also off yaml file for orga metadata

* Update description

* Fix tsvs with correct orga metadata

* Split json template into single and paired reads

* Add template name and version to organisational metadata

* Clean up code and rename file

* Add info about json template files to genomics readme

* Refactor code to review comments

* Spell out cv as controlled_vocabulary

---------

Co-authored-by: Rickard Hammarén <rickard.hammaren@scilifelab.uu.se>
Co-authored-by: Adrien Coulier <adrien.coulier@medsci.uu.se>
</commit_message>
<xml_diff>
--- a/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
+++ b/genomics/ENA_experiment_metadata_fields/ENA_experiment_metadata_template.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="filetype">'cv_run'!$C$1:$C$24</definedName>
-    <definedName name="instrumentmodel">'cv_experiment'!$M$1:$M$83</definedName>
+    <definedName name="instrumentmodel">'cv_experiment'!$M$1:$M$85</definedName>
     <definedName name="libraryselection">'cv_experiment'!$I$1:$I$31</definedName>
     <definedName name="librarysource">'cv_experiment'!$H$1:$H$9</definedName>
     <definedName name="librarystrategy">'cv_experiment'!$G$1:$G$41</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="229">
   <si>
     <t>Instructions how to fill the metadata template</t>
   </si>
@@ -426,6 +426,9 @@
     <t>DNBSEQ-G50</t>
   </si>
   <si>
+    <t>DNBSEQ-T10x4RS</t>
+  </si>
+  <si>
     <t>DNBSEQ-T7</t>
   </si>
   <si>
@@ -505,6 +508,9 @@
   </si>
   <si>
     <t>Illumina NovaSeq X</t>
+  </si>
+  <si>
+    <t>Illumina NovaSeq X Plus</t>
   </si>
   <si>
     <t>Illumina iSeq 100</t>
@@ -1119,7 +1125,7 @@
         <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="150" customHeight="1">
@@ -1160,7 +1166,7 @@
         <v>103</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="G1:M83"/>
+  <dimension ref="G1:M85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1845,6 +1851,16 @@
     </row>
     <row r="83" spans="13:13">
       <c r="M83" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="13:13">
+      <c r="M84" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="13:13">
+      <c r="M85" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1869,57 +1885,57 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="150" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1942,122 +1958,122 @@
   <sheetData>
     <row r="1" spans="3:3">
       <c r="C1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>